<commit_message>
Design Docs, Database, and Exceptions
</commit_message>
<xml_diff>
--- a/Interface_Design/System_External/Requester_and_Ice-Cream_System_Interface_Design.xlsx
+++ b/Interface_Design/System_External/Requester_and_Ice-Cream_System_Interface_Design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\GitHub\Ice-Cream_Repository\Interface_Design\System_External\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFEBB4B-2C4F-4294-A16D-C2FC2DA5B62E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84299D93-D333-4A32-9946-3896320985DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19300" yWindow="60" windowWidth="19060" windowHeight="20670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="70" windowWidth="18920" windowHeight="20780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,20 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Created: 12/26/20 by Tom Lever</t>
   </si>
   <si>
-    <t>Updated: 12/26/20 by Tom Lever</t>
-  </si>
-  <si>
-    <t>From Requester</t>
-  </si>
-  <si>
-    <t>To Requester</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -57,9 +48,6 @@
     <t>Definition</t>
   </si>
   <si>
-    <t>Content Definitions</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -81,9 +69,6 @@
     <t>Product image - Closed</t>
   </si>
   <si>
-    <t>Products</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -138,16 +123,25 @@
     <t>By-ingredient search parameters</t>
   </si>
   <si>
-    <t>Chosen allergens</t>
-  </si>
-  <si>
-    <t>Chosen dietary certifications</t>
-  </si>
-  <si>
-    <t>Chosen sourcing values</t>
-  </si>
-  <si>
-    <t>Info and matching products</t>
+    <t>Info or matching products</t>
+  </si>
+  <si>
+    <t>Inputs from Requester</t>
+  </si>
+  <si>
+    <t>Outputs to Requester</t>
+  </si>
+  <si>
+    <t>Updated: 02/20/21 by Tom Lever</t>
+  </si>
+  <si>
+    <t>Information including "Zero products available" and a reason why zero products are available</t>
+  </si>
+  <si>
+    <t>Matching products</t>
+  </si>
+  <si>
+    <t>Definitions</t>
   </si>
 </sst>
 </file>
@@ -208,11 +202,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -496,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C48"/>
+  <dimension ref="A2:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -509,7 +506,7 @@
   <sheetData>
     <row r="2" spans="1:3" ht="19.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -519,220 +516,212 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B13" s="4"/>
-      <c r="C13" t="s">
-        <v>39</v>
+      <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B22" s="5"/>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B23" s="5"/>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B24" s="5"/>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B25" s="5"/>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B26" s="5"/>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B27" s="5"/>
+      <c r="C27" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="5"/>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B29" s="5"/>
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B30" s="5"/>
+      <c r="C30" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B29" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B31" s="4" t="s">
-        <v>19</v>
+      <c r="B31" t="s">
+        <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B32" s="4"/>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
       <c r="C32" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B33" s="4"/>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
       <c r="C33" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B34" s="4"/>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B35" s="4"/>
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B36" s="4"/>
+      <c r="B36" t="s">
+        <v>23</v>
+      </c>
       <c r="C36" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B37" s="4"/>
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
       <c r="C37" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B38" s="4"/>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
       <c r="C38" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B39" s="4"/>
-      <c r="C39" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B40" s="4"/>
-      <c r="C40" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B41" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B42" t="s">
-        <v>15</v>
-      </c>
-      <c r="C42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B43" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B44" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B45" t="s">
-        <v>24</v>
-      </c>
-      <c r="C45" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B46" t="s">
-        <v>28</v>
-      </c>
-      <c r="C46" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B47" t="s">
         <v>29</v>
       </c>
-      <c r="C47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B48" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" t="s">
-        <v>34</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B31:B40"/>
-    <mergeCell ref="B10:B13"/>
+  <mergeCells count="1">
+    <mergeCell ref="B21:B30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>